<commit_message>
Study of participant 2 completed
</commit_message>
<xml_diff>
--- a/Study1_User2/User2_recognition results.xlsx
+++ b/Study1_User2/User2_recognition results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="-13540" windowWidth="51200" windowHeight="12040" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-13540" windowWidth="51200" windowHeight="10820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="32">
   <si>
     <t>gesture:</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>xrx?y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>xrxx</t>
+  </si>
+  <si>
+    <t>xxx?</t>
+  </si>
+  <si>
+    <t>yry</t>
+  </si>
+  <si>
+    <t>53mm</t>
   </si>
 </sst>
 </file>
@@ -446,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AJ23"/>
+  <dimension ref="A3:AN54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,7 +492,7 @@
     <col min="85" max="85" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -563,7 +578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -680,8 +695,71 @@
       <c r="L5" t="s">
         <v>14</v>
       </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -712,8 +790,71 @@
       <c r="L6" t="s">
         <v>14</v>
       </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,8 +885,71 @@
       <c r="L7" t="s">
         <v>14</v>
       </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -776,8 +980,71 @@
       <c r="L8" t="s">
         <v>14</v>
       </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" t="s">
+        <v>14</v>
+      </c>
+      <c r="W8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -808,8 +1075,71 @@
       <c r="L9" t="s">
         <v>15</v>
       </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" t="s">
+        <v>14</v>
+      </c>
+      <c r="V9" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -840,8 +1170,71 @@
       <c r="L10" t="s">
         <v>15</v>
       </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" t="s">
+        <v>14</v>
+      </c>
+      <c r="V10" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -872,8 +1265,71 @@
       <c r="L11" t="s">
         <v>15</v>
       </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" t="s">
+        <v>14</v>
+      </c>
+      <c r="V11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -904,8 +1360,71 @@
       <c r="L12" t="s">
         <v>13</v>
       </c>
+      <c r="N12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
+      <c r="R12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" t="s">
+        <v>14</v>
+      </c>
+      <c r="T12" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" t="s">
+        <v>14</v>
+      </c>
+      <c r="W12" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -937,7 +1456,7 @@
         <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>16</v>
@@ -991,7 +1510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1135,8 +1654,35 @@
       <c r="X16" t="s">
         <v>14</v>
       </c>
+      <c r="Z16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1194,8 +1740,35 @@
       <c r="X17" t="s">
         <v>26</v>
       </c>
+      <c r="Z17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1253,8 +1826,35 @@
       <c r="X18" t="s">
         <v>14</v>
       </c>
+      <c r="Z18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1312,8 +1912,35 @@
       <c r="X19" t="s">
         <v>14</v>
       </c>
+      <c r="Z19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1371,8 +1998,35 @@
       <c r="X20" t="s">
         <v>15</v>
       </c>
+      <c r="Z20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1430,8 +2084,35 @@
       <c r="X21" t="s">
         <v>22</v>
       </c>
+      <c r="Z21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1489,8 +2170,35 @@
       <c r="X22" t="s">
         <v>14</v>
       </c>
+      <c r="Z22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1547,6 +2255,38 @@
       </c>
       <c r="X23" t="s">
         <v>13</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>